<commit_message>
added presentations to assets spreadsheet
</commit_message>
<xml_diff>
--- a/Package/WATK Assets.xlsx
+++ b/Package/WATK Assets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\sw\dpeted\WindowsAzureTrainingKit\Package\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="335">
   <si>
     <t>Asset</t>
   </si>
@@ -789,6 +789,255 @@
   </si>
   <si>
     <t>Demo-BuildingRealWorldCloudApps</t>
+  </si>
+  <si>
+    <t>PRESENTATION-BuildingAndroidAppsWithWindowsAzureMobileServices</t>
+  </si>
+  <si>
+    <t>PRESENTATION-BuildingAppsWithIaaSAndPaaS</t>
+  </si>
+  <si>
+    <t>PRESENTATION-BuildingDeviceCloudApps</t>
+  </si>
+  <si>
+    <t>PRESENTATION-BuildingiOSAppsWithWindowsAzureMobileServices</t>
+  </si>
+  <si>
+    <t>PRESENTATION-CloudServiceLifecycle</t>
+  </si>
+  <si>
+    <t>PRESENTATION-DeliveringWindows8PushNotifications</t>
+  </si>
+  <si>
+    <t>PRESENTATION-DeployingActiveDirectory</t>
+  </si>
+  <si>
+    <t>PRESENTATION-DeployingSharePointOnVMs</t>
+  </si>
+  <si>
+    <t>PRESENTATION-DeployingSQLServerOnVMs</t>
+  </si>
+  <si>
+    <t>PRESENTATION-DevCamps-CloudServices</t>
+  </si>
+  <si>
+    <t>PRESENTATION-DevCamps-Data</t>
+  </si>
+  <si>
+    <t>PRESENTATION-DevCamps-Keynote</t>
+  </si>
+  <si>
+    <t>PRESENTATION-DevCamps-VirtualMachines</t>
+  </si>
+  <si>
+    <t>PRESENTATION-DevCamps-WebSites</t>
+  </si>
+  <si>
+    <t>PRESENTATION-DevCamps-Windows8AndWindowsAzureWebSites</t>
+  </si>
+  <si>
+    <t>PRESENTATION-DevCamps-WindowsPhoneAndWindowsAzure</t>
+  </si>
+  <si>
+    <t>PRESENTATION-HadoopOnWindowsAzure</t>
+  </si>
+  <si>
+    <t>PRESENTATION-IdentityAndAccessControl</t>
+  </si>
+  <si>
+    <t>PRESENTATION-LinuxVirtualMachines</t>
+  </si>
+  <si>
+    <t>PRESENTATION-ManagingVMsPowerShell</t>
+  </si>
+  <si>
+    <t>PRESENTATION-MigratingAppsAndWorkloads</t>
+  </si>
+  <si>
+    <t>PRESENTATION-ScalableGlobalAndHighlyAvailableApps</t>
+  </si>
+  <si>
+    <t>PRESENTATION-SecurityandIdentity</t>
+  </si>
+  <si>
+    <t>PRESENTATION-SQLDatabase</t>
+  </si>
+  <si>
+    <t>PRESENTATION-SQLDatabaseMigration</t>
+  </si>
+  <si>
+    <t>PRESENTATION-SQLDataSync</t>
+  </si>
+  <si>
+    <t>PRESENTATION-SQLFederation</t>
+  </si>
+  <si>
+    <t>PRESENTATION-SQLReporting</t>
+  </si>
+  <si>
+    <t>PRESENTATION-VirtualMachinesOverview</t>
+  </si>
+  <si>
+    <t>PRESENTATION-VirtualNetworks</t>
+  </si>
+  <si>
+    <t>PRESENTATION-Windows8AndWindowsAzureMobileServices</t>
+  </si>
+  <si>
+    <t>PRESENTATION-Windows8AndWindowsAzureWebSites</t>
+  </si>
+  <si>
+    <t>PRESENTATION-WindowsAzureCloudServices</t>
+  </si>
+  <si>
+    <t>PRESENTATION-WindowsAzureHDInsight</t>
+  </si>
+  <si>
+    <t>PRESENTATION-WindowsAzureITProOverview</t>
+  </si>
+  <si>
+    <t>PRESENTATION-WindowsAzureOverview</t>
+  </si>
+  <si>
+    <t>PRESENTATION-WindowsAzureServiceBus</t>
+  </si>
+  <si>
+    <t>PRESENTATION-WindowsAzureStorage</t>
+  </si>
+  <si>
+    <t>PRESENTATION-WindowsAzureVirtualMachines</t>
+  </si>
+  <si>
+    <t>PRESENTATION-WindowsAzureWebSites</t>
+  </si>
+  <si>
+    <t>PRESENTATION-WindowsPhoneAndWindowsAzureMobileServices</t>
+  </si>
+  <si>
+    <t>BuildingAndroidAppsWithWindowsAzureMobileServices</t>
+  </si>
+  <si>
+    <t>BuildingAppsWithIaaSAndPaaS</t>
+  </si>
+  <si>
+    <t>BuildingDeviceCloudApps</t>
+  </si>
+  <si>
+    <t>BuildingiOSAppsWithWindowsAzureMobileServices</t>
+  </si>
+  <si>
+    <t>CloudServiceLifecycle</t>
+  </si>
+  <si>
+    <t>DeliveringWindows8PushNotifications</t>
+  </si>
+  <si>
+    <t>DeployingActiveDirectory</t>
+  </si>
+  <si>
+    <t>DeployingSharePointOnVMs</t>
+  </si>
+  <si>
+    <t>DeployingSQLServerOnVMs</t>
+  </si>
+  <si>
+    <t>DevCamps-CloudServices</t>
+  </si>
+  <si>
+    <t>DevCamps-Data</t>
+  </si>
+  <si>
+    <t>DevCamps-Keynote</t>
+  </si>
+  <si>
+    <t>DevCamps-VirtualMachines</t>
+  </si>
+  <si>
+    <t>DevCamps-WebSites</t>
+  </si>
+  <si>
+    <t>DevCamps-Windows8AndWindowsAzureWebSites</t>
+  </si>
+  <si>
+    <t>DevCamps-WindowsPhoneAndWindowsAzure</t>
+  </si>
+  <si>
+    <t>HadoopOnWindowsAzure</t>
+  </si>
+  <si>
+    <t>IdentityAndAccessControl</t>
+  </si>
+  <si>
+    <t>LinuxVirtualMachines</t>
+  </si>
+  <si>
+    <t>ManagingVMsPowerShell</t>
+  </si>
+  <si>
+    <t>MigratingAppsAndWorkloads</t>
+  </si>
+  <si>
+    <t>ScalableGlobalAndHighlyAvailableApps</t>
+  </si>
+  <si>
+    <t>SecurityandIdentity</t>
+  </si>
+  <si>
+    <t>SQLDatabase</t>
+  </si>
+  <si>
+    <t>SQLDatabaseMigration</t>
+  </si>
+  <si>
+    <t>SQLDataSync</t>
+  </si>
+  <si>
+    <t>SQLFederation</t>
+  </si>
+  <si>
+    <t>SQLReporting</t>
+  </si>
+  <si>
+    <t>VirtualMachinesOverview</t>
+  </si>
+  <si>
+    <t>VirtualNetworks</t>
+  </si>
+  <si>
+    <t>Windows8AndWindowsAzureMobileServices</t>
+  </si>
+  <si>
+    <t>Windows8AndWindowsAzureWebSites</t>
+  </si>
+  <si>
+    <t>WindowsAzureCloudServices</t>
+  </si>
+  <si>
+    <t>WindowsAzureHDInsight</t>
+  </si>
+  <si>
+    <t>WindowsAzureITProOverview</t>
+  </si>
+  <si>
+    <t>WindowsAzureOverview</t>
+  </si>
+  <si>
+    <t>WindowsAzureServiceBus</t>
+  </si>
+  <si>
+    <t>WindowsAzureStorage</t>
+  </si>
+  <si>
+    <t>WindowsAzureVirtualMachines</t>
+  </si>
+  <si>
+    <t>WindowsAzureWebSites</t>
+  </si>
+  <si>
+    <t>WindowsPhoneAndWindowsAzureMobileServices</t>
+  </si>
+  <si>
+    <t>DevCamps-Windows8AndWindowsAzureMobileServices</t>
   </si>
 </sst>
 </file>
@@ -942,7 +1191,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1035,35 +1284,47 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="36">
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
+        <u/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color auto="1"/>
+        <color theme="10"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -1074,14 +1335,6 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1103,14 +1356,48 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
         <color auto="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1160,6 +1447,36 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1168,10 +1485,10 @@
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="10"/>
+        <sz val="11"/>
+        <color theme="0"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
@@ -1181,17 +1498,7 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1224,6 +1531,56 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1493,6 +1850,108 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
@@ -1568,7 +2027,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I76" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I76" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31">
   <autoFilter ref="A1:I76">
     <filterColumn colId="2">
       <customFilters>
@@ -1580,36 +2039,52 @@
     <sortCondition ref="A1:A76"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" name="P" dataDxfId="21"/>
-    <tableColumn id="2" name="Asset" dataDxfId="5" dataCellStyle="Hyperlink"/>
-    <tableColumn id="9" name="VSO" dataDxfId="3" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" name="SDK" dataDxfId="4"/>
-    <tableColumn id="4" name="In WATK" dataDxfId="20"/>
-    <tableColumn id="5" name="VS" dataDxfId="19"/>
-    <tableColumn id="6" name="OS" dataDxfId="18"/>
-    <tableColumn id="7" name="Last Update" dataDxfId="17"/>
-    <tableColumn id="8" name="Notes" dataDxfId="16"/>
+    <tableColumn id="1" name="P" dataDxfId="30"/>
+    <tableColumn id="2" name="Asset" dataDxfId="29" dataCellStyle="Hyperlink"/>
+    <tableColumn id="9" name="VSO" dataDxfId="28" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" name="SDK" dataDxfId="27"/>
+    <tableColumn id="4" name="In WATK" dataDxfId="26"/>
+    <tableColumn id="5" name="VS" dataDxfId="25"/>
+    <tableColumn id="6" name="OS" dataDxfId="24"/>
+    <tableColumn id="7" name="Last Update" dataDxfId="23"/>
+    <tableColumn id="8" name="Notes" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I34" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I34" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
   <autoFilter ref="A1:I34"/>
   <sortState ref="A2:I34">
     <sortCondition ref="A1:A34"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" name="P" dataDxfId="11"/>
-    <tableColumn id="2" name="Asset" dataDxfId="2"/>
-    <tableColumn id="9" name="VSO" dataDxfId="0" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" name="SDK" dataDxfId="1"/>
-    <tableColumn id="4" name="In WATK" dataDxfId="10"/>
-    <tableColumn id="5" name="VS" dataDxfId="9"/>
-    <tableColumn id="6" name="OS" dataDxfId="8"/>
-    <tableColumn id="7" name="Last Update" dataDxfId="7"/>
-    <tableColumn id="8" name="Notes" dataDxfId="6"/>
+    <tableColumn id="1" name="P" dataDxfId="17"/>
+    <tableColumn id="2" name="Asset" dataDxfId="16"/>
+    <tableColumn id="9" name="VSO" dataDxfId="15" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" name="SDK" dataDxfId="14"/>
+    <tableColumn id="4" name="In WATK" dataDxfId="13"/>
+    <tableColumn id="5" name="VS" dataDxfId="12"/>
+    <tableColumn id="6" name="OS" dataDxfId="11"/>
+    <tableColumn id="7" name="Last Update" dataDxfId="10"/>
+    <tableColumn id="8" name="Notes" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:D46" totalsRowShown="0" headerRowDxfId="8" dataDxfId="1" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:D46"/>
+  <sortState ref="A2:D46">
+    <sortCondition ref="B1:B46"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" name="P" dataDxfId="4"/>
+    <tableColumn id="2" name="Asset" dataDxfId="0" dataCellStyle="Hyperlink"/>
+    <tableColumn id="9" name="VSO" dataDxfId="3" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" name="In WATK" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1882,7 +2357,7 @@
   <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4038,7 +4513,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5019,12 +5494,571 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="34" t="s">
+        <v>293</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" t="s">
+        <v>294</v>
+      </c>
+      <c r="C4" t="s">
+        <v>253</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C5" t="s">
+        <v>254</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" t="s">
+        <v>296</v>
+      </c>
+      <c r="C6" t="s">
+        <v>255</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="34" t="s">
+        <v>296</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" t="s">
+        <v>297</v>
+      </c>
+      <c r="C8" t="s">
+        <v>256</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" t="s">
+        <v>298</v>
+      </c>
+      <c r="C9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" t="s">
+        <v>299</v>
+      </c>
+      <c r="C10" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" t="s">
+        <v>300</v>
+      </c>
+      <c r="C11" t="s">
+        <v>259</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" t="s">
+        <v>301</v>
+      </c>
+      <c r="C12" t="s">
+        <v>260</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" t="s">
+        <v>302</v>
+      </c>
+      <c r="C13" t="s">
+        <v>261</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" t="s">
+        <v>303</v>
+      </c>
+      <c r="C14" t="s">
+        <v>262</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" t="s">
+        <v>304</v>
+      </c>
+      <c r="C15" t="s">
+        <v>263</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" t="s">
+        <v>305</v>
+      </c>
+      <c r="C16" t="s">
+        <v>264</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" t="s">
+        <v>306</v>
+      </c>
+      <c r="C17" t="s">
+        <v>265</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="34" t="s">
+        <v>334</v>
+      </c>
+      <c r="C18" s="35"/>
+      <c r="D18" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" t="s">
+        <v>307</v>
+      </c>
+      <c r="C19" t="s">
+        <v>266</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" t="s">
+        <v>308</v>
+      </c>
+      <c r="C20" t="s">
+        <v>267</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" t="s">
+        <v>309</v>
+      </c>
+      <c r="C21" t="s">
+        <v>268</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" t="s">
+        <v>310</v>
+      </c>
+      <c r="C22" t="s">
+        <v>269</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" t="s">
+        <v>311</v>
+      </c>
+      <c r="C23" t="s">
+        <v>270</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" t="s">
+        <v>312</v>
+      </c>
+      <c r="C24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" t="s">
+        <v>313</v>
+      </c>
+      <c r="C25" t="s">
+        <v>272</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" t="s">
+        <v>314</v>
+      </c>
+      <c r="C26" t="s">
+        <v>273</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" t="s">
+        <v>315</v>
+      </c>
+      <c r="C27" t="s">
+        <v>274</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" t="s">
+        <v>316</v>
+      </c>
+      <c r="C28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" t="s">
+        <v>317</v>
+      </c>
+      <c r="C29" t="s">
+        <v>276</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" t="s">
+        <v>318</v>
+      </c>
+      <c r="C30" t="s">
+        <v>277</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" t="s">
+        <v>319</v>
+      </c>
+      <c r="C31" t="s">
+        <v>278</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" t="s">
+        <v>320</v>
+      </c>
+      <c r="C32" t="s">
+        <v>279</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" t="s">
+        <v>321</v>
+      </c>
+      <c r="C33" t="s">
+        <v>280</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" t="s">
+        <v>322</v>
+      </c>
+      <c r="C34" t="s">
+        <v>281</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" t="s">
+        <v>323</v>
+      </c>
+      <c r="C35" t="s">
+        <v>282</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="34" t="s">
+        <v>323</v>
+      </c>
+      <c r="C36" s="35"/>
+      <c r="D36" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" t="s">
+        <v>324</v>
+      </c>
+      <c r="C37" t="s">
+        <v>283</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="34" t="s">
+        <v>325</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="34" t="s">
+        <v>326</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="34" t="s">
+        <v>327</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="34" t="s">
+        <v>328</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="34" t="s">
+        <v>329</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="34" t="s">
+        <v>330</v>
+      </c>
+      <c r="C43" s="36" t="s">
+        <v>289</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44" s="34" t="s">
+        <v>331</v>
+      </c>
+      <c r="C44" s="36" t="s">
+        <v>290</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="34" t="s">
+        <v>332</v>
+      </c>
+      <c r="C45" s="36" t="s">
+        <v>291</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="26"/>
+      <c r="B46" s="34" t="s">
+        <v>333</v>
+      </c>
+      <c r="C46" s="37" t="s">
+        <v>292</v>
+      </c>
+      <c r="D46" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed duplicated presentations from WATK assets
</commit_message>
<xml_diff>
--- a/Package/WATK Assets.xlsx
+++ b/Package/WATK Assets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7305"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7305" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Labs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="335">
   <si>
     <t>Asset</t>
   </si>
@@ -1304,48 +1304,6 @@
   <dxfs count="36">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="10"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1414,6 +1372,40 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1455,13 +1447,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -1471,6 +1456,21 @@
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
@@ -2075,16 +2075,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:D46" totalsRowShown="0" headerRowDxfId="8" dataDxfId="1" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
-  <autoFilter ref="A1:D46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:D43" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:D43"/>
   <sortState ref="A2:D46">
     <sortCondition ref="B1:B46"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="P" dataDxfId="4"/>
-    <tableColumn id="2" name="Asset" dataDxfId="0" dataCellStyle="Hyperlink"/>
-    <tableColumn id="9" name="VSO" dataDxfId="3" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" name="In WATK" dataDxfId="2"/>
+    <tableColumn id="1" name="P" dataDxfId="3"/>
+    <tableColumn id="2" name="Asset" dataDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="9" name="VSO" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" name="In WATK" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2356,7 +2356,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -5494,10 +5494,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5537,10 +5537,12 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="34" t="s">
-        <v>293</v>
-      </c>
-      <c r="C3" s="35"/>
+      <c r="B3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C3" t="s">
+        <v>253</v>
+      </c>
       <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
@@ -5548,10 +5550,10 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>9</v>
@@ -5560,10 +5562,10 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>9</v>
@@ -5572,21 +5574,23 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C6" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="34" t="s">
-        <v>296</v>
-      </c>
-      <c r="C7" s="35"/>
+      <c r="B7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C7" t="s">
+        <v>257</v>
+      </c>
       <c r="D7" s="5" t="s">
         <v>9</v>
       </c>
@@ -5594,22 +5598,22 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C8" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>9</v>
@@ -5618,10 +5622,10 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C10" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>9</v>
@@ -5630,10 +5634,10 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C11" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>9</v>
@@ -5642,10 +5646,10 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C12" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>9</v>
@@ -5654,10 +5658,10 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C13" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>9</v>
@@ -5666,10 +5670,10 @@
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C14" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>9</v>
@@ -5678,10 +5682,10 @@
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C15" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>9</v>
@@ -5689,12 +5693,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" t="s">
-        <v>305</v>
-      </c>
-      <c r="C16" t="s">
-        <v>264</v>
-      </c>
+      <c r="B16" s="34" t="s">
+        <v>334</v>
+      </c>
+      <c r="C16" s="35"/>
       <c r="D16" s="5" t="s">
         <v>9</v>
       </c>
@@ -5702,10 +5704,10 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C17" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>9</v>
@@ -5713,10 +5715,12 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="34" t="s">
-        <v>334</v>
-      </c>
-      <c r="C18" s="35"/>
+      <c r="B18" t="s">
+        <v>308</v>
+      </c>
+      <c r="C18" t="s">
+        <v>267</v>
+      </c>
       <c r="D18" s="5" t="s">
         <v>9</v>
       </c>
@@ -5724,10 +5728,10 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C19" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>9</v>
@@ -5736,10 +5740,10 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C20" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>9</v>
@@ -5748,10 +5752,10 @@
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C21" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>9</v>
@@ -5760,10 +5764,10 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C22" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>9</v>
@@ -5772,10 +5776,10 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C23" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>9</v>
@@ -5784,10 +5788,10 @@
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C24" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>9</v>
@@ -5796,22 +5800,22 @@
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C25" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C26" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>9</v>
@@ -5820,22 +5824,22 @@
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C27" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C28" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>9</v>
@@ -5844,10 +5848,10 @@
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C29" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>9</v>
@@ -5856,10 +5860,10 @@
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C30" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>9</v>
@@ -5868,22 +5872,22 @@
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C31" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C32" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>9</v>
@@ -5892,22 +5896,22 @@
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C33" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C34" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>9</v>
@@ -5915,11 +5919,11 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
-      <c r="B35" t="s">
-        <v>323</v>
-      </c>
-      <c r="C35" t="s">
-        <v>282</v>
+      <c r="B35" s="34" t="s">
+        <v>325</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>284</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>9</v>
@@ -5928,20 +5932,22 @@
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="34" t="s">
-        <v>323</v>
-      </c>
-      <c r="C36" s="35"/>
+        <v>326</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>285</v>
+      </c>
       <c r="D36" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" t="s">
-        <v>324</v>
-      </c>
-      <c r="C37" t="s">
-        <v>283</v>
+      <c r="B37" s="34" t="s">
+        <v>327</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>286</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>9</v>
@@ -5950,10 +5956,10 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="34" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="C38" s="34" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>9</v>
@@ -5962,10 +5968,10 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="34" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="C39" s="34" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>9</v>
@@ -5974,10 +5980,10 @@
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="34" t="s">
-        <v>327</v>
-      </c>
-      <c r="C40" s="34" t="s">
-        <v>286</v>
+        <v>330</v>
+      </c>
+      <c r="C40" s="36" t="s">
+        <v>289</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>9</v>
@@ -5986,10 +5992,10 @@
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="34" t="s">
-        <v>328</v>
-      </c>
-      <c r="C41" s="34" t="s">
-        <v>287</v>
+        <v>331</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>290</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>9</v>
@@ -5998,60 +6004,24 @@
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="34" t="s">
-        <v>329</v>
-      </c>
-      <c r="C42" s="34" t="s">
-        <v>288</v>
+        <v>332</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>291</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="34" t="s">
-        <v>330</v>
-      </c>
-      <c r="C43" s="36" t="s">
-        <v>289</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="34" t="s">
-        <v>331</v>
-      </c>
-      <c r="C44" s="36" t="s">
-        <v>290</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="34" t="s">
-        <v>332</v>
-      </c>
-      <c r="C45" s="36" t="s">
-        <v>291</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
-      <c r="B46" s="34" t="s">
         <v>333</v>
       </c>
-      <c r="C46" s="37" t="s">
+      <c r="C43" s="37" t="s">
         <v>292</v>
       </c>
-      <c r="D46" s="26" t="s">
+      <c r="D43" s="26" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>